<commit_message>
Change order actions and sort orders by date
</commit_message>
<xml_diff>
--- a/usuarios-TIME.xlsx
+++ b/usuarios-TIME.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESCRITORIO\TaxiMoto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6807E1C6-05D7-4C00-A646-65B8B04F76BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FBBA4E-49C7-43DE-B22E-408A6CA2AE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26985" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="112">
   <si>
     <t>3496-461432</t>
   </si>
@@ -354,13 +354,28 @@
   </si>
   <si>
     <t>Garcia</t>
+  </si>
+  <si>
+    <t>Pizza Days</t>
+  </si>
+  <si>
+    <t>Sarmiento 2057</t>
+  </si>
+  <si>
+    <t>[-31.44904338194299, -60.93138958233732]</t>
+  </si>
+  <si>
+    <t>pizzadays</t>
+  </si>
+  <si>
+    <t>pizzadays2057</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,6 +419,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -446,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -476,9 +497,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -799,7 +817,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,12 +1089,22 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="A14" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -1105,9 +1133,9 @@
       <c r="F16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="17"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>91</v>
       </c>
@@ -1126,9 +1154,8 @@
       <c r="F17" s="6">
         <v>32749190</v>
       </c>
-      <c r="G17" s="15"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>92</v>
       </c>
@@ -1147,9 +1174,8 @@
       <c r="F18" s="9">
         <v>41406385</v>
       </c>
-      <c r="G18" s="15"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>96</v>
       </c>
@@ -1168,9 +1194,8 @@
       <c r="F19" s="6">
         <v>35139824</v>
       </c>
-      <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>88</v>
       </c>
@@ -1189,9 +1214,8 @@
       <c r="F20" s="6">
         <v>39854464</v>
       </c>
-      <c r="G20" s="15"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>94</v>
       </c>
@@ -1210,9 +1234,8 @@
       <c r="F21" s="9">
         <v>43769540</v>
       </c>
-      <c r="G21" s="15"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>86</v>
       </c>
@@ -1231,9 +1254,8 @@
       <c r="F22" s="9">
         <v>44307445</v>
       </c>
-      <c r="G22" s="15"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>100</v>
       </c>
@@ -1252,9 +1274,8 @@
       <c r="F23" s="9">
         <v>41514940</v>
       </c>
-      <c r="G23" s="15"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>102</v>
       </c>
@@ -1273,9 +1294,8 @@
       <c r="F24" s="6">
         <v>42531953</v>
       </c>
-      <c r="G24" s="15"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>104</v>
       </c>
@@ -1294,20 +1314,13 @@
       <c r="F25" s="6">
         <v>37564534</v>
       </c>
-      <c r="G25" s="15"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="15"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="18"/>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="16"/>
-      <c r="G28" s="15"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="15"/>
+      <c r="F26" s="15"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="15"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
@@ -1337,6 +1350,7 @@
       <c r="A43" s="13"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>